<commit_message>
Created the complete generalInfo table and added the R script for creating this table
</commit_message>
<xml_diff>
--- a/codeBook.xlsx
+++ b/codeBook.xlsx
@@ -45,7 +45,7 @@
     <t>imdbRating</t>
   </si>
   <si>
-    <t>"The Gang Gets Racist"</t>
+    <t>EpiLength</t>
   </si>
 </sst>
 </file>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -432,7 +432,7 @@
     <col min="9" max="12" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,19 +457,43 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created template for recording episode data and worked on adding to the codeBook
</commit_message>
<xml_diff>
--- a/codeBook.xlsx
+++ b/codeBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27920" yWindow="-10760" windowWidth="35960" windowHeight="18180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="generalInfo" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="399">
   <si>
     <t>AbsOrder</t>
   </si>
@@ -1221,13 +1221,79 @@
   </si>
   <si>
     <t>Patriotism</t>
+  </si>
+  <si>
+    <t>NightCrawl</t>
+  </si>
+  <si>
+    <t>DeeCar</t>
+  </si>
+  <si>
+    <t>MacKarate</t>
+  </si>
+  <si>
+    <t>DeeTurkey</t>
+  </si>
+  <si>
+    <t>NightDayMan</t>
+  </si>
+  <si>
+    <t>BlackFace</t>
+  </si>
+  <si>
+    <t>CharlieIlliteracy</t>
+  </si>
+  <si>
+    <t>OcularPat</t>
+  </si>
+  <si>
+    <t>FrankViet</t>
+  </si>
+  <si>
+    <t>GodDamn</t>
+  </si>
+  <si>
+    <t>Acapella</t>
+  </si>
+  <si>
+    <t>DennisSex</t>
+  </si>
+  <si>
+    <t>OpBadass</t>
+  </si>
+  <si>
+    <t>UncleJackHands</t>
+  </si>
+  <si>
+    <t>BirdLaw</t>
+  </si>
+  <si>
+    <t>CharlieLawyer</t>
+  </si>
+  <si>
+    <t>PhilSports</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>CharlieWork</t>
+  </si>
+  <si>
+    <t>DeeActor</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1245,6 +1311,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Menlo Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Menlo Regular"/>
       <family val="2"/>
     </font>
@@ -1266,7 +1338,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1298,15 +1370,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1322,6 +1411,14 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1337,6 +1434,14 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1677,7 +1782,7 @@
   <dimension ref="A1:K114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5699,7 +5804,7 @@
   <dimension ref="A1:AJ114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6176,7 +6281,109 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
         <v>0</v>
       </c>
     </row>
@@ -6747,22 +6954,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM114"/>
+  <dimension ref="A1:BG114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM1" sqref="AM1"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
     <col min="12" max="21" width="12.125" customWidth="1"/>
+    <col min="27" max="27" width="13.25" customWidth="1"/>
     <col min="28" max="30" width="19.875" customWidth="1"/>
+    <col min="31" max="31" width="18.5" customWidth="1"/>
     <col min="32" max="32" width="13.125" customWidth="1"/>
+    <col min="33" max="40" width="13.5" customWidth="1"/>
+    <col min="41" max="41" width="16.5" customWidth="1"/>
+    <col min="42" max="59" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:59">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6826,132 +7038,366 @@
       <c r="U1" t="s">
         <v>358</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="AC1" t="s">
         <v>364</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>365</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>366</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>368</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>369</v>
       </c>
       <c r="AG1" t="s">
         <v>370</v>
       </c>
       <c r="AH1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>375</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>377</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>380</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>381</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>383</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>384</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>385</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>388</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>390</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>391</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>394</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AX1" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AY1" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>373</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>374</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>375</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="BA1" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="BD1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>392</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:59">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:59">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:59">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:39">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>397</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>397</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>397</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="AZ5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BF5" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:59">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:59">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:59">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:59">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:59">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:59">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:59">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:59">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:59">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:59">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7448,6 +7894,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>